<commit_message>
feat: :bug: Conexion DB
Conexion DB
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="301">
   <si>
     <t xml:space="preserve">              CONTRATO DE COMPRAVENTA DE UN VEHÍCULO </t>
   </si>
@@ -1354,6 +1354,66 @@
   </si>
   <si>
     <t>2345</t>
+  </si>
+  <si>
+    <t>gfdsg</t>
+  </si>
+  <si>
+    <t>gsfdg</t>
+  </si>
+  <si>
+    <t>sdfg</t>
+  </si>
+  <si>
+    <t>fdsg</t>
+  </si>
+  <si>
+    <t>4frg</t>
+  </si>
+  <si>
+    <t>fdsf</t>
+  </si>
+  <si>
+    <t>sfg</t>
+  </si>
+  <si>
+    <t>789</t>
+  </si>
+  <si>
+    <t>0987</t>
+  </si>
+  <si>
+    <t>654</t>
+  </si>
+  <si>
+    <t>321</t>
+  </si>
+  <si>
+    <t>bastog</t>
+  </si>
+  <si>
+    <t>juna jose</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>456</t>
+  </si>
+  <si>
+    <t>qwer</t>
+  </si>
+  <si>
+    <t>qwre</t>
+  </si>
+  <si>
+    <t>987</t>
+  </si>
+  <si>
+    <t>JUAN</t>
+  </si>
+  <si>
+    <t>JOSE</t>
   </si>
 </sst>
 </file>
@@ -5253,12 +5313,12 @@
       </c>
       <c r="V7" s="57"/>
       <c r="W7" s="62" t="s">
-        <v>279</v>
+        <v>300</v>
       </c>
       <c r="X7" s="62"/>
       <c r="Y7" s="62"/>
       <c r="Z7" s="75" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="AA7" s="75"/>
       <c r="AB7" s="75"/>
@@ -5782,7 +5842,7 @@
       <c r="AC17" s="78"/>
       <c r="AD17" s="57"/>
       <c r="AE17" s="93" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="AF17" s="93"/>
       <c r="AG17" s="93"/>
@@ -5876,7 +5936,7 @@
       <c r="U19" s="89"/>
       <c r="V19" s="57"/>
       <c r="W19" s="62" t="s">
-        <v>274</v>
+        <v>295</v>
       </c>
       <c r="X19" s="62"/>
       <c r="Y19" s="62"/>
@@ -5886,7 +5946,7 @@
       <c r="AC19" s="62"/>
       <c r="AD19" s="57"/>
       <c r="AE19" s="62" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="AF19" s="62"/>
       <c r="AG19" s="62"/>
@@ -6015,7 +6075,7 @@
       <c r="AC22" s="71"/>
       <c r="AD22" s="57"/>
       <c r="AE22" s="62" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="AF22" s="62"/>
       <c r="AG22" s="62"/>
@@ -6127,7 +6187,7 @@
       <c r="AC24" s="104"/>
       <c r="AD24" s="106"/>
       <c r="AE24" s="107" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="AF24" s="107"/>
       <c r="AG24" s="107"/>
@@ -6941,7 +7001,7 @@
       <c r="U41" s="112"/>
       <c r="V41" s="57"/>
       <c r="W41" s="85" t="s">
-        <v>277</v>
+        <v>298</v>
       </c>
       <c r="X41" s="85"/>
       <c r="Y41" s="85"/>

</xml_diff>